<commit_message>
Update part numbers and silkscreen
</commit_message>
<xml_diff>
--- a/Hardware Files/Fabrication Files/8BitWiFiVisualizer_BOM.xlsx
+++ b/Hardware Files/Fabrication Files/8BitWiFiVisualizer_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mccocz\Designs\Stasis Electronics\Projects\8BitWiFiVisualizer\Hardware Files\Fabrication Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C44CA7-4A08-4BF4-9BD0-7B09EE4AE249}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBCA52C-9292-4A4F-9E46-C5A9EA2E7624}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{72C8A0F0-9BB1-4DEB-B051-62D0D80A5C1E}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
   <si>
     <t>References</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>MINTRON</t>
+  </si>
+  <si>
+    <t>QTY per 100</t>
   </si>
 </sst>
 </file>
@@ -339,7 +342,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -376,8 +382,8 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{80BB34B6-CA13-4B24-AA2C-4EE331A28642}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="10">
-    <queryTableFields count="8">
+  <queryTableRefresh nextId="11" unboundColumnsRight="1">
+    <queryTableFields count="9">
       <queryTableField id="1" name="Component" tableColumnId="1"/>
       <queryTableField id="2" name="References" tableColumnId="2"/>
       <queryTableField id="3" name="Value" tableColumnId="3"/>
@@ -386,6 +392,7 @@
       <queryTableField id="6" name="Manufacturer" tableColumnId="6"/>
       <queryTableField id="7" name="Manufacturer PN" tableColumnId="7"/>
       <queryTableField id="8" name="Quantity Per PCB" tableColumnId="8"/>
+      <queryTableField id="10" dataBound="0" tableColumnId="10"/>
     </queryTableFields>
     <queryTableDeletedFields count="1">
       <deletedField name="Datasheet"/>
@@ -395,17 +402,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92BBB22C-C1EC-4A8D-9007-8909215E06EE}" name="_8Bit_WiFi_Visualizer_bom_A04" displayName="_8Bit_WiFi_Visualizer_bom_A04" ref="A1:H12" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H12" xr:uid="{E2E8B100-49AF-4894-9C9E-7D502A5971C2}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{3B314D00-7AFC-4774-A35E-585B6F3FCA62}" uniqueName="1" name="Component" queryTableFieldId="1" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{F5124DA9-1CE3-47DF-8B4F-EE806FE87D3B}" uniqueName="2" name="References" queryTableFieldId="2" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{E4B8E2D5-8A46-4496-ACA2-B37C50E840F1}" uniqueName="3" name="Value" queryTableFieldId="3" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{8B9764FA-1DD4-4E05-9B82-B1FB96F710F9}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{2BFEE474-4A05-40E1-83D5-80B21BD81ECF}" uniqueName="5" name="LCSC Order Number" queryTableFieldId="5" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{C2E1EF82-C981-4AD1-AC0C-205346100DC0}" uniqueName="6" name="Manufacturer" queryTableFieldId="6" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{18192DC0-236F-4FCB-96BF-DBEE7DD7FE7E}" uniqueName="7" name="Manufacturer PN" queryTableFieldId="7" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{92BBB22C-C1EC-4A8D-9007-8909215E06EE}" name="_8Bit_WiFi_Visualizer_bom_A04" displayName="_8Bit_WiFi_Visualizer_bom_A04" ref="A1:I12" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:I12" xr:uid="{E2E8B100-49AF-4894-9C9E-7D502A5971C2}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{3B314D00-7AFC-4774-A35E-585B6F3FCA62}" uniqueName="1" name="Component" queryTableFieldId="1" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{F5124DA9-1CE3-47DF-8B4F-EE806FE87D3B}" uniqueName="2" name="References" queryTableFieldId="2" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{E4B8E2D5-8A46-4496-ACA2-B37C50E840F1}" uniqueName="3" name="Value" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{8B9764FA-1DD4-4E05-9B82-B1FB96F710F9}" uniqueName="4" name="Description" queryTableFieldId="4" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{2BFEE474-4A05-40E1-83D5-80B21BD81ECF}" uniqueName="5" name="LCSC Order Number" queryTableFieldId="5" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{C2E1EF82-C981-4AD1-AC0C-205346100DC0}" uniqueName="6" name="Manufacturer" queryTableFieldId="6" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{18192DC0-236F-4FCB-96BF-DBEE7DD7FE7E}" uniqueName="7" name="Manufacturer PN" queryTableFieldId="7" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{1B9994AD-9D87-4ACB-910B-1EE402839A5E}" uniqueName="8" name="Quantity Per PCB" queryTableFieldId="8"/>
+    <tableColumn id="10" xr3:uid="{301581AF-E611-4579-ACAC-E27B3FCED487}" uniqueName="10" name="QTY per 100" queryTableFieldId="10" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -708,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F566BE4B-F45C-46EA-B9EA-3C8DCF0DA188}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -724,9 +732,10 @@
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -751,8 +760,11 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -777,8 +789,11 @@
       <c r="H2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="1">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -803,8 +818,11 @@
       <c r="H3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
@@ -829,8 +847,11 @@
       <c r="H4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="1">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>27</v>
       </c>
@@ -855,8 +876,11 @@
       <c r="H5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -881,8 +905,11 @@
       <c r="H6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>38</v>
       </c>
@@ -907,8 +934,11 @@
       <c r="H7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="1">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>45</v>
       </c>
@@ -933,8 +963,11 @@
       <c r="H8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -959,8 +992,11 @@
       <c r="H9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>58</v>
       </c>
@@ -985,8 +1021,11 @@
       <c r="H10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>65</v>
       </c>
@@ -1011,8 +1050,11 @@
       <c r="H11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>72</v>
       </c>
@@ -1036,6 +1078,9 @@
       </c>
       <c r="H12">
         <v>1</v>
+      </c>
+      <c r="I12" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.25">

</xml_diff>